<commit_message>
agregue reporte pdf ventas en inventario
</commit_message>
<xml_diff>
--- a/src/main/resources/static/uploads/reportes/reporte_inventario.xlsx
+++ b/src/main/resources/static/uploads/reportes/reporte_inventario.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ID</t>
   </si>
@@ -26,19 +26,25 @@
     <t>Stock</t>
   </si>
   <si>
-    <t>Cama de perro</t>
-  </si>
-  <si>
-    <t>Collar para gatos</t>
-  </si>
-  <si>
-    <t>Premio de perro</t>
-  </si>
-  <si>
-    <t>Rascador para gato</t>
-  </si>
-  <si>
-    <t>Plato de comida</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Adult Cat</t>
+  </si>
+  <si>
+    <t>Aloe Vera Shampoo Dog &amp; Cat 500 ml</t>
+  </si>
+  <si>
+    <t>Brit Pate &amp; Meat Salmon 800 Gr</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -91,14 +97,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="2.71875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="16.34375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="31.203125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="6.0625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="5.3984375" customWidth="true" bestFit="true"/>
   </cols>
@@ -125,10 +131,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>60.0</v>
+        <v>0.05</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>10.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="3">
@@ -139,10 +145,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>13.0</v>
+        <v>15.0</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>15.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="4">
@@ -153,10 +159,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>16.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="5">
@@ -167,10 +173,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>70.0</v>
+        <v>138.0</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>6.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="6">
@@ -181,10 +187,38 @@
         <v>8</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>14.0</v>
+        <v>53.0</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>18.0</v>
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>13.0</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>16.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>